<commit_message>
update results with full workloads' results
</commit_message>
<xml_diff>
--- a/project-acn/results/Results.xlsx
+++ b/project-acn/results/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\SSgumS\Downloads\Compressed\cloudsimsdn\project-acn\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B7AB9652-CBCB-4578-8E52-B55CDEF9193D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68BA1DAD-93DB-4FE5-B3CE-32A2E88B0B9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="37710" windowHeight="16440" xr2:uid="{8AEF8FF4-CBA6-4DBF-8F82-DF1A8EA55659}"/>
   </bookViews>
@@ -55,7 +55,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -63,13 +66,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -81,13 +96,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -303,10 +323,10 @@
             <c:numRef>
               <c:f>Sheet1!$B$2</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1.41</c:v>
+                  <c:v>0.97331189884895597</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -441,10 +461,10 @@
             <c:numRef>
               <c:f>Sheet1!$C$2</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>13.7</c:v>
+                  <c:v>9.7855404994651298</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -579,10 +599,10 @@
             <c:numRef>
               <c:f>Sheet1!$D$2</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>22.68</c:v>
+                  <c:v>4.9203750281142797</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -977,7 +997,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1298,13 +1318,13 @@
             <c:numRef>
               <c:f>Sheet1!$B$3:$B$4</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>0.03</c:v>
+                <c:pt idx="0" formatCode="0.00">
+                  <c:v>2.7555473982924999E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.32</c:v>
+                  <c:v>0.208883632233589</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1442,13 +1462,13 @@
             <c:numRef>
               <c:f>Sheet1!$C$3:$C$4</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>0.03</c:v>
+                <c:pt idx="0" formatCode="0.00">
+                  <c:v>2.76004301943347E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.39</c:v>
+                  <c:v>2.4118845871233399</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1586,13 +1606,13 @@
             <c:numRef>
               <c:f>Sheet1!$D$3:$D$4</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>0.03</c:v>
+                <c:pt idx="0" formatCode="0.00">
+                  <c:v>2.6525640041961299E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.63</c:v>
+                  <c:v>1.1969367069761001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2032,7 +2052,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3650,13 +3670,13 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" customWidth="1"/>
     <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
@@ -3673,10 +3693,10 @@
       <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3684,19 +3704,19 @@
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2">
-        <v>1.41</v>
+      <c r="B2" s="1">
+        <v>0.97331189884895597</v>
       </c>
-      <c r="C2">
-        <v>13.7</v>
+      <c r="C2" s="1">
+        <v>9.7855404994651298</v>
       </c>
-      <c r="D2">
-        <v>22.68</v>
+      <c r="D2" s="1">
+        <v>4.9203750281142797</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="3">
         <v>24.69</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="3">
         <v>0.79</v>
       </c>
     </row>
@@ -3704,19 +3724,19 @@
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="2">
+        <v>2.7555473982924999E-2</v>
+      </c>
+      <c r="C3" s="2">
+        <v>2.76004301943347E-2</v>
+      </c>
+      <c r="D3" s="2">
+        <v>2.6525640041961299E-2</v>
+      </c>
+      <c r="E3" s="3">
         <v>0.03</v>
       </c>
-      <c r="C3">
-        <v>0.03</v>
-      </c>
-      <c r="D3">
-        <v>0.03</v>
-      </c>
-      <c r="E3">
-        <v>0.03</v>
-      </c>
-      <c r="F3">
+      <c r="F3" s="3">
         <v>0.03</v>
       </c>
     </row>
@@ -3724,19 +3744,19 @@
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4">
-        <v>0.32</v>
+      <c r="B4" s="1">
+        <v>0.208883632233589</v>
       </c>
-      <c r="C4">
-        <v>3.39</v>
+      <c r="C4" s="1">
+        <v>2.4118845871233399</v>
       </c>
-      <c r="D4">
-        <v>5.63</v>
+      <c r="D4" s="1">
+        <v>1.1969367069761001</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="3">
         <v>6.14</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="3">
         <v>0.16</v>
       </c>
     </row>

</xml_diff>